<commit_message>
Slått sammen nye datasett til et datasett
</commit_message>
<xml_diff>
--- a/Arbeidsledighet.xlsx
+++ b/Arbeidsledighet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfa6bab4499e8cf7/Dokumenter/DEV/MSB104_Ass1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{74B81493-EE9D-440C-82DC-C8ABE903383C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91D3F5BD-61CE-4BD9-974C-2B2D59CF414E}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{74B81493-EE9D-440C-82DC-C8ABE903383C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B91440B-D453-4234-9F7E-78EB605CA65C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="112">
   <si>
     <t>Unemployment rates by educational attainment level and NUTS 2 region [lfst_r_lfu3rt__custom_18862746]</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t xml:space="preserve">Arbeidsledighet </t>
+  </si>
+  <si>
+    <t>nuts2</t>
   </si>
 </sst>
 </file>
@@ -377,27 +380,32 @@
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color indexed="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -579,6 +587,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1056,7 +1068,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1068,7 +1080,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>30</v>

</xml_diff>